<commit_message>
Added point anomalies with noise analysis to excel
</commit_message>
<xml_diff>
--- a/HMMs analysis.xlsx
+++ b/HMMs analysis.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexis/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexis/Desktop/csec-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="38320" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -216,19 +216,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -287,45 +274,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -371,19 +319,6 @@
         <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -437,21 +372,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -545,6 +465,30 @@
       </left>
       <right/>
       <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -558,7 +502,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -578,88 +522,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -671,19 +612,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
@@ -692,19 +639,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -986,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:V51"/>
+  <dimension ref="B1:W51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1001,96 +939,96 @@
     <col min="15" max="15" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="19" t="s">
+    <row r="1" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="21"/>
+      <c r="D2" s="43"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="18" t="s">
+      <c r="Q2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-    </row>
-    <row r="3" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23" t="s">
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+    </row>
+    <row r="3" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="21" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="17"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="40"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="15" t="s">
+      <c r="Q3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="17"/>
-    </row>
-    <row r="4" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="40"/>
+    </row>
+    <row r="4" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9">
         <v>2</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>-926607.9</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="15">
         <v>-5292092</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="29">
+      <c r="H4" s="18">
         <v>0.5</v>
       </c>
-      <c r="I4" s="24">
+      <c r="I4" s="13">
         <v>1</v>
       </c>
-      <c r="J4" s="24">
+      <c r="J4" s="13">
         <v>1.25</v>
       </c>
-      <c r="K4" s="24">
+      <c r="K4" s="13">
         <v>1.5</v>
       </c>
-      <c r="L4" s="24">
+      <c r="L4" s="13">
         <v>1.75</v>
       </c>
-      <c r="M4" s="25">
+      <c r="M4" s="14">
         <v>2</v>
       </c>
       <c r="N4" s="1"/>
@@ -1117,23 +1055,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C5" s="46">
         <v>-566751.5</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="25">
         <v>-4693582</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="34" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="9">
         <v>2</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="19">
         <v>46513</v>
       </c>
       <c r="I5" s="9">
@@ -1148,38 +1086,38 @@
       <c r="L5" s="9">
         <v>4174</v>
       </c>
-      <c r="M5" s="26">
+      <c r="M5" s="15">
         <v>2905</v>
       </c>
       <c r="N5" s="1"/>
-      <c r="O5" s="35" t="s">
+      <c r="O5" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="11">
+      <c r="P5" s="10">
         <v>2</v>
       </c>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="28"/>
-    </row>
-    <row r="6" spans="2:22" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+    </row>
+    <row r="6" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8">
         <v>4</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="8">
         <v>-419092.2</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="16">
         <v>-4149228</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="35"/>
       <c r="G6" s="7">
         <v>3</v>
       </c>
-      <c r="H6" s="49">
+      <c r="H6" s="33">
         <v>29374</v>
       </c>
       <c r="I6" s="7">
@@ -1194,107 +1132,137 @@
       <c r="L6" s="7">
         <v>1580</v>
       </c>
-      <c r="M6" s="41">
+      <c r="M6" s="25">
         <v>1117</v>
       </c>
       <c r="N6" s="1"/>
-      <c r="O6" s="36"/>
+      <c r="O6" s="35"/>
       <c r="P6" s="7">
         <v>3</v>
       </c>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="41"/>
-    </row>
-    <row r="7" spans="2:22" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q6" s="7">
+        <v>43713</v>
+      </c>
+      <c r="R6" s="7">
+        <v>20852</v>
+      </c>
+      <c r="S6" s="7">
+        <v>15572</v>
+      </c>
+      <c r="T6" s="7">
+        <v>12169</v>
+      </c>
+      <c r="U6" s="7">
+        <v>9594</v>
+      </c>
+      <c r="V6" s="7">
+        <v>8213</v>
+      </c>
+      <c r="W6" s="47">
+        <v>15524</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="7">
+      <c r="F7" s="36"/>
+      <c r="G7" s="23">
         <v>4</v>
       </c>
-      <c r="H7" s="49">
+      <c r="H7" s="44">
         <v>24026</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="23">
         <v>6981</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="23">
         <v>4546</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="23">
         <v>2921</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="23">
         <v>1978</v>
       </c>
-      <c r="M7" s="41">
+      <c r="M7" s="26">
         <v>1409</v>
       </c>
       <c r="N7" s="1"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="39">
+      <c r="O7" s="35"/>
+      <c r="P7" s="23">
         <v>4</v>
       </c>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="39"/>
-      <c r="T7" s="39"/>
-      <c r="U7" s="39"/>
-      <c r="V7" s="42"/>
-    </row>
-    <row r="8" spans="2:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q7" s="23">
+        <v>39448</v>
+      </c>
+      <c r="R7" s="23">
+        <v>19581</v>
+      </c>
+      <c r="S7" s="23">
+        <v>15632</v>
+      </c>
+      <c r="T7" s="23">
+        <v>12573</v>
+      </c>
+      <c r="U7" s="23">
+        <v>10222</v>
+      </c>
+      <c r="V7" s="23">
+        <v>8711</v>
+      </c>
+      <c r="W7" s="1">
+        <v>15587</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="10">
         <v>2</v>
       </c>
-      <c r="H8" s="49">
+      <c r="H8" s="45">
         <v>46876</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="10">
         <v>23683</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="10">
         <v>13050</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="10">
         <v>6360</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="10">
         <v>4477</v>
       </c>
-      <c r="M8" s="41">
+      <c r="M8" s="17">
         <v>3324</v>
       </c>
       <c r="N8" s="1"/>
-      <c r="O8" s="35" t="s">
+      <c r="O8" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="P8" s="11">
+      <c r="P8" s="10">
         <v>2</v>
       </c>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="28"/>
-    </row>
-    <row r="9" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F9" s="36"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+    </row>
+    <row r="9" spans="2:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F9" s="35"/>
       <c r="G9" s="7">
         <v>3</v>
       </c>
-      <c r="H9" s="49">
+      <c r="H9" s="33">
         <v>46516</v>
       </c>
       <c r="I9" s="7">
@@ -1309,27 +1277,42 @@
       <c r="L9" s="7">
         <v>4464</v>
       </c>
-      <c r="M9" s="41">
+      <c r="M9" s="25">
         <v>1930</v>
       </c>
       <c r="N9" s="1"/>
-      <c r="O9" s="36"/>
+      <c r="O9" s="35"/>
       <c r="P9" s="7">
         <v>3</v>
       </c>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="41"/>
-    </row>
-    <row r="10" spans="2:22" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F10" s="37"/>
+      <c r="Q9" s="7">
+        <v>57858</v>
+      </c>
+      <c r="R9" s="7">
+        <v>29482</v>
+      </c>
+      <c r="S9" s="7">
+        <v>23066</v>
+      </c>
+      <c r="T9" s="7">
+        <v>19166</v>
+      </c>
+      <c r="U9" s="7">
+        <v>14309</v>
+      </c>
+      <c r="V9" s="7">
+        <v>10790</v>
+      </c>
+      <c r="W9" s="1">
+        <v>15367</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="36"/>
       <c r="G10" s="8">
         <v>4</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="11">
         <v>42863</v>
       </c>
       <c r="I10" s="8">
@@ -1344,11 +1327,11 @@
       <c r="L10" s="8">
         <v>5674</v>
       </c>
-      <c r="M10" s="27">
+      <c r="M10" s="16">
         <v>3052</v>
       </c>
       <c r="N10" s="1"/>
-      <c r="O10" s="37"/>
+      <c r="O10" s="36"/>
       <c r="P10" s="8">
         <v>4</v>
       </c>
@@ -1357,9 +1340,9 @@
       <c r="S10" s="8"/>
       <c r="T10" s="8"/>
       <c r="U10" s="8"/>
-      <c r="V10" s="27"/>
-    </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V10" s="8"/>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.2">
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1378,7 +1361,7 @@
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.2">
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1397,7 +1380,7 @@
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.2">
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1416,96 +1399,96 @@
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
     </row>
-    <row r="14" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-      <c r="Q14" s="18" t="s">
+      <c r="Q14" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
+      <c r="R14" s="37"/>
+      <c r="S14" s="37"/>
+      <c r="T14" s="37"/>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
     </row>
-    <row r="15" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
-      <c r="Q15" s="19" t="s">
+      <c r="Q15" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="R15" s="20"/>
-      <c r="S15" s="20"/>
-      <c r="T15" s="21"/>
+      <c r="R15" s="42"/>
+      <c r="S15" s="42"/>
+      <c r="T15" s="43"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
     </row>
-    <row r="16" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F16" s="1"/>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="H16" s="24">
+      <c r="H16" s="13">
         <v>5</v>
       </c>
-      <c r="I16" s="24">
+      <c r="I16" s="13">
         <v>10</v>
       </c>
-      <c r="J16" s="24">
+      <c r="J16" s="13">
         <v>15</v>
       </c>
-      <c r="K16" s="25">
+      <c r="K16" s="14">
         <v>20</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="23" t="s">
+      <c r="P16" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="Q16" s="24">
+      <c r="Q16" s="13">
         <v>5</v>
       </c>
-      <c r="R16" s="48">
+      <c r="R16" s="32">
         <v>10</v>
       </c>
-      <c r="S16" s="24">
+      <c r="S16" s="13">
         <v>15</v>
       </c>
-      <c r="T16" s="24">
+      <c r="T16" s="13">
         <v>20</v>
       </c>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
     </row>
     <row r="17" spans="6:22" x14ac:dyDescent="0.2">
-      <c r="F17" s="35" t="s">
+      <c r="F17" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="40">
+      <c r="G17" s="24">
         <v>2</v>
       </c>
       <c r="H17" s="9">
@@ -1517,27 +1500,27 @@
       <c r="J17" s="9">
         <v>755</v>
       </c>
-      <c r="K17" s="26">
+      <c r="K17" s="15">
         <v>453</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="1"/>
-      <c r="O17" s="35" t="s">
+      <c r="O17" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="P17" s="40">
+      <c r="P17" s="24">
         <v>2</v>
       </c>
       <c r="Q17" s="9"/>
-      <c r="R17" s="43"/>
+      <c r="R17" s="27"/>
       <c r="S17" s="9"/>
       <c r="T17" s="9"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
     </row>
     <row r="18" spans="6:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F18" s="36"/>
+      <c r="F18" s="35"/>
       <c r="G18" s="7">
         <v>3</v>
       </c>
@@ -1550,91 +1533,91 @@
       <c r="J18" s="7">
         <v>213</v>
       </c>
-      <c r="K18" s="41">
+      <c r="K18" s="25">
         <v>124</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="1"/>
-      <c r="O18" s="36"/>
+      <c r="O18" s="35"/>
       <c r="P18" s="7">
         <v>3</v>
       </c>
       <c r="Q18" s="7"/>
-      <c r="R18" s="44"/>
+      <c r="R18" s="28"/>
       <c r="S18" s="7"/>
       <c r="T18" s="7"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
     </row>
     <row r="19" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F19" s="36"/>
-      <c r="G19" s="39">
+      <c r="F19" s="35"/>
+      <c r="G19" s="23">
         <v>4</v>
       </c>
-      <c r="H19" s="39">
+      <c r="H19" s="23">
         <v>1067</v>
       </c>
-      <c r="I19" s="39">
+      <c r="I19" s="23">
         <v>322</v>
       </c>
-      <c r="J19" s="39">
+      <c r="J19" s="23">
         <v>213</v>
       </c>
-      <c r="K19" s="42">
+      <c r="K19" s="26">
         <v>123</v>
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="1"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="39">
+      <c r="O19" s="35"/>
+      <c r="P19" s="23">
         <v>4</v>
       </c>
-      <c r="Q19" s="39"/>
-      <c r="R19" s="45"/>
-      <c r="S19" s="39"/>
-      <c r="T19" s="39"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
     </row>
     <row r="20" spans="6:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="35" t="s">
+      <c r="F20" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="10">
         <v>2</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="10">
         <v>4369</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="10">
         <v>1858</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="10">
         <v>1284</v>
       </c>
-      <c r="K20" s="28">
+      <c r="K20" s="17">
         <v>900</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="1"/>
-      <c r="O20" s="35" t="s">
+      <c r="O20" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="P20" s="11">
+      <c r="P20" s="10">
         <v>2</v>
       </c>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="46"/>
-      <c r="S20" s="11"/>
-      <c r="T20" s="11"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
     </row>
     <row r="21" spans="6:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="36"/>
+      <c r="F21" s="35"/>
       <c r="G21" s="7">
         <v>3</v>
       </c>
@@ -1647,25 +1630,25 @@
       <c r="J21" s="7">
         <v>886</v>
       </c>
-      <c r="K21" s="41">
+      <c r="K21" s="25">
         <v>577</v>
       </c>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="1"/>
-      <c r="O21" s="36"/>
+      <c r="O21" s="35"/>
       <c r="P21" s="7">
         <v>3</v>
       </c>
       <c r="Q21" s="7"/>
-      <c r="R21" s="44"/>
+      <c r="R21" s="28"/>
       <c r="S21" s="7"/>
       <c r="T21" s="7"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
     </row>
     <row r="22" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F22" s="37"/>
+      <c r="F22" s="36"/>
       <c r="G22" s="8">
         <v>4</v>
       </c>
@@ -1678,18 +1661,18 @@
       <c r="J22" s="8">
         <v>944</v>
       </c>
-      <c r="K22" s="27">
+      <c r="K22" s="16">
         <v>625</v>
       </c>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
       <c r="N22" s="1"/>
-      <c r="O22" s="37"/>
+      <c r="O22" s="36"/>
       <c r="P22" s="8">
         <v>4</v>
       </c>
       <c r="Q22" s="8"/>
-      <c r="R22" s="47"/>
+      <c r="R22" s="31"/>
       <c r="S22" s="8"/>
       <c r="T22" s="8"/>
       <c r="U22" s="1"/>
@@ -1793,98 +1776,98 @@
     <row r="28" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="18" t="s">
+      <c r="H28" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="37"/>
+      <c r="M28" s="37"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
-      <c r="Q28" s="18" t="s">
+      <c r="Q28" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="R28" s="18"/>
-      <c r="S28" s="18"/>
-      <c r="T28" s="18"/>
-      <c r="U28" s="18"/>
-      <c r="V28" s="18"/>
+      <c r="R28" s="37"/>
+      <c r="S28" s="37"/>
+      <c r="T28" s="37"/>
+      <c r="U28" s="37"/>
+      <c r="V28" s="37"/>
     </row>
     <row r="29" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="15" t="s">
+      <c r="H29" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="17"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="40"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
-      <c r="Q29" s="15" t="s">
+      <c r="Q29" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="R29" s="16"/>
-      <c r="S29" s="16"/>
-      <c r="T29" s="16"/>
-      <c r="U29" s="16"/>
-      <c r="V29" s="17"/>
+      <c r="R29" s="39"/>
+      <c r="S29" s="39"/>
+      <c r="T29" s="39"/>
+      <c r="U29" s="39"/>
+      <c r="V29" s="40"/>
     </row>
     <row r="30" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F30" s="1"/>
-      <c r="G30" s="23" t="s">
+      <c r="G30" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="H30" s="24">
+      <c r="H30" s="13">
         <v>0.5</v>
       </c>
-      <c r="I30" s="24">
+      <c r="I30" s="13">
         <v>1</v>
       </c>
-      <c r="J30" s="24">
+      <c r="J30" s="13">
         <v>1.25</v>
       </c>
-      <c r="K30" s="25">
+      <c r="K30" s="14">
         <v>1.5</v>
       </c>
-      <c r="L30" s="24">
+      <c r="L30" s="13">
         <v>1.75</v>
       </c>
-      <c r="M30" s="24">
+      <c r="M30" s="13">
         <v>2</v>
       </c>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
-      <c r="P30" s="23" t="s">
+      <c r="P30" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="Q30" s="24">
+      <c r="Q30" s="13">
         <v>0.5</v>
       </c>
-      <c r="R30" s="48">
+      <c r="R30" s="32">
         <v>1</v>
       </c>
-      <c r="S30" s="24">
+      <c r="S30" s="13">
         <v>1.25</v>
       </c>
-      <c r="T30" s="48">
+      <c r="T30" s="32">
         <v>1.5</v>
       </c>
-      <c r="U30" s="24">
+      <c r="U30" s="13">
         <v>1.75</v>
       </c>
-      <c r="V30" s="24">
+      <c r="V30" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="6:22" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F31" s="35" t="s">
+      <c r="F31" s="34" t="s">
         <v>1</v>
       </c>
       <c r="G31" s="9">
@@ -1899,7 +1882,7 @@
       <c r="J31" s="9">
         <v>128317</v>
       </c>
-      <c r="K31" s="11">
+      <c r="K31" s="10">
         <v>81922</v>
       </c>
       <c r="L31" s="9">
@@ -1909,7 +1892,7 @@
         <v>29992</v>
       </c>
       <c r="N31" s="1"/>
-      <c r="O31" s="35" t="s">
+      <c r="O31" s="34" t="s">
         <v>1</v>
       </c>
       <c r="P31" s="9">
@@ -1918,13 +1901,13 @@
       <c r="Q31" s="9">
         <v>278173</v>
       </c>
-      <c r="R31" s="43">
+      <c r="R31" s="27">
         <v>168466</v>
       </c>
       <c r="S31" s="9">
         <v>127756</v>
       </c>
-      <c r="T31" s="43">
+      <c r="T31" s="27">
         <v>81756</v>
       </c>
       <c r="U31" s="9">
@@ -1935,7 +1918,7 @@
       </c>
     </row>
     <row r="32" spans="6:22" x14ac:dyDescent="0.2">
-      <c r="F32" s="36"/>
+      <c r="F32" s="35"/>
       <c r="G32" s="7">
         <v>3</v>
       </c>
@@ -1958,20 +1941,20 @@
         <v>22857</v>
       </c>
       <c r="N32" s="1"/>
-      <c r="O32" s="36"/>
+      <c r="O32" s="35"/>
       <c r="P32" s="7">
         <v>3</v>
       </c>
       <c r="Q32" s="7">
         <v>225136</v>
       </c>
-      <c r="R32" s="44">
+      <c r="R32" s="28">
         <v>109950</v>
       </c>
       <c r="S32" s="7">
         <v>71031</v>
       </c>
-      <c r="T32" s="44">
+      <c r="T32" s="28">
         <v>46213</v>
       </c>
       <c r="U32" s="7">
@@ -1982,105 +1965,105 @@
       </c>
     </row>
     <row r="33" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F33" s="36"/>
-      <c r="G33" s="39">
+      <c r="F33" s="35"/>
+      <c r="G33" s="23">
         <v>4</v>
       </c>
-      <c r="H33" s="39">
+      <c r="H33" s="23">
         <v>229259</v>
       </c>
-      <c r="I33" s="39">
+      <c r="I33" s="23">
         <v>113768</v>
       </c>
-      <c r="J33" s="39">
+      <c r="J33" s="23">
         <v>81357</v>
       </c>
-      <c r="K33" s="39">
+      <c r="K33" s="23">
         <v>55863</v>
       </c>
-      <c r="L33" s="39">
+      <c r="L33" s="23">
         <v>38301</v>
       </c>
-      <c r="M33" s="39">
+      <c r="M33" s="23">
         <v>29090</v>
       </c>
       <c r="N33" s="1"/>
-      <c r="O33" s="36"/>
-      <c r="P33" s="39">
+      <c r="O33" s="35"/>
+      <c r="P33" s="23">
         <v>4</v>
       </c>
-      <c r="Q33" s="39">
+      <c r="Q33" s="23">
         <v>229471</v>
       </c>
-      <c r="R33" s="45">
+      <c r="R33" s="29">
         <v>114166</v>
       </c>
-      <c r="S33" s="39">
+      <c r="S33" s="23">
         <v>81432</v>
       </c>
-      <c r="T33" s="45">
+      <c r="T33" s="29">
         <v>55911</v>
       </c>
-      <c r="U33" s="39">
+      <c r="U33" s="23">
         <v>38499</v>
       </c>
-      <c r="V33" s="39">
+      <c r="V33" s="23">
         <v>29451</v>
       </c>
     </row>
     <row r="34" spans="6:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F34" s="35" t="s">
+      <c r="F34" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="G34" s="11">
+      <c r="G34" s="10">
         <v>2</v>
       </c>
-      <c r="H34" s="11">
+      <c r="H34" s="10">
         <v>225391</v>
       </c>
-      <c r="I34" s="11">
+      <c r="I34" s="10">
         <v>106804</v>
       </c>
-      <c r="J34" s="11">
+      <c r="J34" s="10">
         <v>71287</v>
       </c>
-      <c r="K34" s="11">
+      <c r="K34" s="10">
         <v>40329</v>
       </c>
-      <c r="L34" s="11">
+      <c r="L34" s="10">
         <v>21574</v>
       </c>
-      <c r="M34" s="11">
+      <c r="M34" s="10">
         <v>14893</v>
       </c>
       <c r="N34" s="1"/>
-      <c r="O34" s="35" t="s">
+      <c r="O34" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="P34" s="11">
+      <c r="P34" s="10">
         <v>2</v>
       </c>
-      <c r="Q34" s="11">
+      <c r="Q34" s="10">
         <v>219643</v>
       </c>
-      <c r="R34" s="46">
+      <c r="R34" s="30">
         <v>101425</v>
       </c>
-      <c r="S34" s="11">
+      <c r="S34" s="10">
         <v>67468</v>
       </c>
-      <c r="T34" s="46">
+      <c r="T34" s="30">
         <v>38747</v>
       </c>
-      <c r="U34" s="11">
+      <c r="U34" s="10">
         <v>21461</v>
       </c>
-      <c r="V34" s="11">
+      <c r="V34" s="10">
         <v>15020</v>
       </c>
     </row>
     <row r="35" spans="6:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F35" s="36"/>
+      <c r="F35" s="35"/>
       <c r="G35" s="7">
         <v>3</v>
       </c>
@@ -2103,20 +2086,20 @@
         <v>11659</v>
       </c>
       <c r="N35" s="2"/>
-      <c r="O35" s="36"/>
+      <c r="O35" s="35"/>
       <c r="P35" s="7">
         <v>3</v>
       </c>
       <c r="Q35" s="7">
         <v>203468</v>
       </c>
-      <c r="R35" s="44">
+      <c r="R35" s="28">
         <v>91604</v>
       </c>
       <c r="S35" s="7">
         <v>55595</v>
       </c>
-      <c r="T35" s="44">
+      <c r="T35" s="28">
         <v>35527</v>
       </c>
       <c r="U35" s="7">
@@ -2127,7 +2110,7 @@
       </c>
     </row>
     <row r="36" spans="6:22" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F36" s="37"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="8">
         <v>4</v>
       </c>
@@ -2150,20 +2133,20 @@
         <v>10564</v>
       </c>
       <c r="N36" s="2"/>
-      <c r="O36" s="37"/>
+      <c r="O36" s="36"/>
       <c r="P36" s="8">
         <v>4</v>
       </c>
       <c r="Q36" s="8">
         <v>207083</v>
       </c>
-      <c r="R36" s="47">
+      <c r="R36" s="31">
         <v>77387</v>
       </c>
       <c r="S36" s="8">
         <v>46808</v>
       </c>
-      <c r="T36" s="47">
+      <c r="T36" s="31">
         <v>28886</v>
       </c>
       <c r="U36" s="8">
@@ -2233,93 +2216,93 @@
     <row r="40" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="18" t="s">
+      <c r="H40" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18"/>
-      <c r="K40" s="18"/>
-      <c r="L40" s="31"/>
-      <c r="M40" s="31"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="37"/>
+      <c r="K40" s="37"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
-      <c r="Q40" s="18" t="s">
+      <c r="Q40" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
-      <c r="T40" s="18"/>
-      <c r="U40" s="31"/>
-      <c r="V40" s="31"/>
+      <c r="R40" s="37"/>
+      <c r="S40" s="37"/>
+      <c r="T40" s="37"/>
+      <c r="U40" s="20"/>
+      <c r="V40" s="20"/>
     </row>
     <row r="41" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="19" t="s">
+      <c r="H41" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="21"/>
-      <c r="L41" s="31"/>
-      <c r="M41" s="31"/>
+      <c r="I41" s="42"/>
+      <c r="J41" s="42"/>
+      <c r="K41" s="43"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
-      <c r="Q41" s="19" t="s">
+      <c r="Q41" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="R41" s="20"/>
-      <c r="S41" s="20"/>
-      <c r="T41" s="21"/>
-      <c r="U41" s="31"/>
-      <c r="V41" s="31"/>
+      <c r="R41" s="42"/>
+      <c r="S41" s="42"/>
+      <c r="T41" s="43"/>
+      <c r="U41" s="20"/>
+      <c r="V41" s="20"/>
     </row>
     <row r="42" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F42" s="1"/>
       <c r="G42" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H42" s="24">
+      <c r="H42" s="13">
         <v>5</v>
       </c>
-      <c r="I42" s="24">
+      <c r="I42" s="13">
         <v>10</v>
       </c>
-      <c r="J42" s="24">
+      <c r="J42" s="13">
         <v>15</v>
       </c>
-      <c r="K42" s="25">
+      <c r="K42" s="14">
         <v>20</v>
       </c>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
-      <c r="P42" s="23" t="s">
+      <c r="P42" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="Q42" s="25">
+      <c r="Q42" s="14">
         <v>5</v>
       </c>
-      <c r="R42" s="29">
+      <c r="R42" s="18">
         <v>10</v>
       </c>
-      <c r="S42" s="24">
+      <c r="S42" s="13">
         <v>15</v>
       </c>
-      <c r="T42" s="24">
+      <c r="T42" s="13">
         <v>20</v>
       </c>
       <c r="U42" s="4"/>
       <c r="V42" s="4"/>
     </row>
     <row r="43" spans="6:22" x14ac:dyDescent="0.2">
-      <c r="F43" s="35" t="s">
+      <c r="F43" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="G43" s="38">
+      <c r="G43" s="22">
         <v>2</v>
       </c>
       <c r="H43" s="9">
@@ -2337,16 +2320,16 @@
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
       <c r="N43" s="1"/>
-      <c r="O43" s="35" t="s">
+      <c r="O43" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="P43" s="40">
+      <c r="P43" s="24">
         <v>2</v>
       </c>
-      <c r="Q43" s="43">
+      <c r="Q43" s="27">
         <v>29557</v>
       </c>
-      <c r="R43" s="11">
+      <c r="R43" s="10">
         <v>10555</v>
       </c>
       <c r="S43" s="9">
@@ -2359,7 +2342,7 @@
       <c r="V43" s="4"/>
     </row>
     <row r="44" spans="6:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F44" s="36"/>
+      <c r="F44" s="35"/>
       <c r="G44" s="7">
         <v>3</v>
       </c>
@@ -2378,11 +2361,11 @@
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
       <c r="N44" s="1"/>
-      <c r="O44" s="36"/>
+      <c r="O44" s="35"/>
       <c r="P44" s="7">
         <v>3</v>
       </c>
-      <c r="Q44" s="44">
+      <c r="Q44" s="28">
         <v>15604</v>
       </c>
       <c r="R44" s="7">
@@ -2398,89 +2381,89 @@
       <c r="V44" s="4"/>
     </row>
     <row r="45" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F45" s="36"/>
-      <c r="G45" s="39">
+      <c r="F45" s="35"/>
+      <c r="G45" s="23">
         <v>4</v>
       </c>
-      <c r="H45" s="39">
+      <c r="H45" s="23">
         <v>17232</v>
       </c>
-      <c r="I45" s="39">
+      <c r="I45" s="23">
         <v>5089</v>
       </c>
-      <c r="J45" s="39">
+      <c r="J45" s="23">
         <v>3445</v>
       </c>
-      <c r="K45" s="39">
+      <c r="K45" s="23">
         <v>1746</v>
       </c>
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
       <c r="N45" s="1"/>
-      <c r="O45" s="36"/>
-      <c r="P45" s="39">
+      <c r="O45" s="35"/>
+      <c r="P45" s="23">
         <v>4</v>
       </c>
-      <c r="Q45" s="45">
+      <c r="Q45" s="29">
         <v>17232</v>
       </c>
-      <c r="R45" s="39">
+      <c r="R45" s="23">
         <v>5089</v>
       </c>
-      <c r="S45" s="39">
+      <c r="S45" s="23">
         <v>3445</v>
       </c>
-      <c r="T45" s="39">
+      <c r="T45" s="23">
         <v>1746</v>
       </c>
       <c r="U45" s="4"/>
       <c r="V45" s="4"/>
     </row>
     <row r="46" spans="6:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F46" s="35" t="s">
+      <c r="F46" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="G46" s="11">
+      <c r="G46" s="10">
         <v>2</v>
       </c>
-      <c r="H46" s="11">
+      <c r="H46" s="10">
         <v>14764</v>
       </c>
-      <c r="I46" s="11">
+      <c r="I46" s="10">
         <v>4694</v>
       </c>
-      <c r="J46" s="11">
+      <c r="J46" s="10">
         <v>3259</v>
       </c>
-      <c r="K46" s="11">
+      <c r="K46" s="10">
         <v>1960</v>
       </c>
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
       <c r="N46" s="1"/>
-      <c r="O46" s="35" t="s">
+      <c r="O46" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="P46" s="11">
+      <c r="P46" s="10">
         <v>2</v>
       </c>
-      <c r="Q46" s="46">
+      <c r="Q46" s="30">
         <v>13519</v>
       </c>
-      <c r="R46" s="11">
+      <c r="R46" s="10">
         <v>4090</v>
       </c>
-      <c r="S46" s="11">
+      <c r="S46" s="10">
         <v>2814</v>
       </c>
-      <c r="T46" s="11">
+      <c r="T46" s="10">
         <v>1624</v>
       </c>
       <c r="U46" s="4"/>
       <c r="V46" s="4"/>
     </row>
     <row r="47" spans="6:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F47" s="36"/>
+      <c r="F47" s="35"/>
       <c r="G47" s="7">
         <v>3</v>
       </c>
@@ -2499,11 +2482,11 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
       <c r="N47" s="1"/>
-      <c r="O47" s="36"/>
+      <c r="O47" s="35"/>
       <c r="P47" s="7">
         <v>3</v>
       </c>
-      <c r="Q47" s="44">
+      <c r="Q47" s="28">
         <v>10331</v>
       </c>
       <c r="R47" s="7">
@@ -2519,7 +2502,7 @@
       <c r="V47" s="4"/>
     </row>
     <row r="48" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F48" s="37"/>
+      <c r="F48" s="36"/>
       <c r="G48" s="8">
         <v>4</v>
       </c>
@@ -2538,11 +2521,11 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="1"/>
-      <c r="O48" s="37"/>
+      <c r="O48" s="36"/>
       <c r="P48" s="8">
         <v>4</v>
       </c>
-      <c r="Q48" s="47">
+      <c r="Q48" s="31">
         <v>6580</v>
       </c>
       <c r="R48" s="8">
@@ -2616,12 +2599,15 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="O17:O19"/>
-    <mergeCell ref="O20:O22"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="O8:O10"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="Q2:V2"/>
+    <mergeCell ref="Q3:V3"/>
+    <mergeCell ref="Q14:T14"/>
+    <mergeCell ref="Q15:T15"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
     <mergeCell ref="O43:O45"/>
     <mergeCell ref="O46:O48"/>
     <mergeCell ref="F43:F45"/>
@@ -2638,17 +2624,14 @@
     <mergeCell ref="H29:M29"/>
     <mergeCell ref="F34:F36"/>
     <mergeCell ref="F31:F33"/>
+    <mergeCell ref="O17:O19"/>
+    <mergeCell ref="O20:O22"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="O8:O10"/>
     <mergeCell ref="F17:F19"/>
-    <mergeCell ref="Q2:V2"/>
-    <mergeCell ref="Q3:V3"/>
-    <mergeCell ref="Q14:T14"/>
-    <mergeCell ref="Q15:T15"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
     <mergeCell ref="F20:F22"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="H3:M3"/>
-    <mergeCell ref="H2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finished filling out excel spreadsheet
</commit_message>
<xml_diff>
--- a/HMMs analysis.xlsx
+++ b/HMMs analysis.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexis/Desktop/csec-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matheson/Dropbox/School/Summer 2017/CMPT 318/Project/csec-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="38320" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="33520" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -603,6 +603,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -611,39 +644,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -926,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -941,31 +941,31 @@
   <sheetData>
     <row r="1" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="43"/>
+      <c r="D2" s="39"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="37" t="s">
+      <c r="Q2" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
     </row>
     <row r="3" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -979,25 +979,25 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="40"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="42"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="38" t="s">
+      <c r="Q3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="40"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="42"/>
     </row>
     <row r="4" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9">
@@ -1059,13 +1059,13 @@
       <c r="B5" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="36">
         <v>-566751.5</v>
       </c>
       <c r="D5" s="25">
         <v>-4693582</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F5" s="45" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="9">
@@ -1090,18 +1090,30 @@
         <v>2905</v>
       </c>
       <c r="N5" s="1"/>
-      <c r="O5" s="34" t="s">
+      <c r="O5" s="45" t="s">
         <v>1</v>
       </c>
       <c r="P5" s="10">
         <v>2</v>
       </c>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
+      <c r="Q5" s="10">
+        <v>59064</v>
+      </c>
+      <c r="R5" s="10">
+        <v>31048</v>
+      </c>
+      <c r="S5" s="10">
+        <v>23239</v>
+      </c>
+      <c r="T5" s="10">
+        <v>17031</v>
+      </c>
+      <c r="U5" s="10">
+        <v>11585</v>
+      </c>
+      <c r="V5" s="10">
+        <v>9246</v>
+      </c>
     </row>
     <row r="6" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8">
@@ -1113,7 +1125,7 @@
       <c r="D6" s="16">
         <v>-4149228</v>
       </c>
-      <c r="F6" s="35"/>
+      <c r="F6" s="46"/>
       <c r="G6" s="7">
         <v>3</v>
       </c>
@@ -1136,7 +1148,7 @@
         <v>1117</v>
       </c>
       <c r="N6" s="1"/>
-      <c r="O6" s="35"/>
+      <c r="O6" s="46"/>
       <c r="P6" s="7">
         <v>3</v>
       </c>
@@ -1158,7 +1170,7 @@
       <c r="V6" s="7">
         <v>8213</v>
       </c>
-      <c r="W6" s="47">
+      <c r="W6" s="37">
         <v>15524</v>
       </c>
     </row>
@@ -1166,11 +1178,11 @@
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="F7" s="36"/>
+      <c r="F7" s="47"/>
       <c r="G7" s="23">
         <v>4</v>
       </c>
-      <c r="H7" s="44">
+      <c r="H7" s="34">
         <v>24026</v>
       </c>
       <c r="I7" s="23">
@@ -1189,7 +1201,7 @@
         <v>1409</v>
       </c>
       <c r="N7" s="1"/>
-      <c r="O7" s="35"/>
+      <c r="O7" s="46"/>
       <c r="P7" s="23">
         <v>4</v>
       </c>
@@ -1219,13 +1231,13 @@
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="46" t="s">
         <v>5</v>
       </c>
       <c r="G8" s="10">
         <v>2</v>
       </c>
-      <c r="H8" s="45">
+      <c r="H8" s="35">
         <v>46876</v>
       </c>
       <c r="I8" s="10">
@@ -1244,21 +1256,33 @@
         <v>3324</v>
       </c>
       <c r="N8" s="1"/>
-      <c r="O8" s="34" t="s">
+      <c r="O8" s="45" t="s">
         <v>5</v>
       </c>
       <c r="P8" s="10">
         <v>2</v>
       </c>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
+      <c r="Q8" s="10">
+        <v>57438</v>
+      </c>
+      <c r="R8" s="10">
+        <v>34935</v>
+      </c>
+      <c r="S8" s="10">
+        <v>24086</v>
+      </c>
+      <c r="T8" s="10">
+        <v>16903</v>
+      </c>
+      <c r="U8" s="10">
+        <v>14571</v>
+      </c>
+      <c r="V8" s="10">
+        <v>12960</v>
+      </c>
     </row>
     <row r="9" spans="2:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F9" s="35"/>
+      <c r="F9" s="46"/>
       <c r="G9" s="7">
         <v>3</v>
       </c>
@@ -1281,7 +1305,7 @@
         <v>1930</v>
       </c>
       <c r="N9" s="1"/>
-      <c r="O9" s="35"/>
+      <c r="O9" s="46"/>
       <c r="P9" s="7">
         <v>3</v>
       </c>
@@ -1308,7 +1332,7 @@
       </c>
     </row>
     <row r="10" spans="2:23" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F10" s="36"/>
+      <c r="F10" s="47"/>
       <c r="G10" s="8">
         <v>4</v>
       </c>
@@ -1331,16 +1355,28 @@
         <v>3052</v>
       </c>
       <c r="N10" s="1"/>
-      <c r="O10" s="36"/>
+      <c r="O10" s="47"/>
       <c r="P10" s="8">
         <v>4</v>
       </c>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
+      <c r="Q10" s="8">
+        <v>54919</v>
+      </c>
+      <c r="R10" s="8">
+        <v>30045</v>
+      </c>
+      <c r="S10" s="8">
+        <v>23262</v>
+      </c>
+      <c r="T10" s="8">
+        <v>19491</v>
+      </c>
+      <c r="U10" s="8">
+        <v>16167</v>
+      </c>
+      <c r="V10" s="8">
+        <v>12532</v>
+      </c>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.2">
       <c r="F11" s="1"/>
@@ -1402,46 +1438,46 @@
     <row r="14" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="37" t="s">
+      <c r="H14" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-      <c r="Q14" s="37" t="s">
+      <c r="Q14" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="R14" s="37"/>
-      <c r="S14" s="37"/>
-      <c r="T14" s="37"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="43"/>
+      <c r="T14" s="43"/>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
     </row>
     <row r="15" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="41" t="s">
+      <c r="H15" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="43"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="39"/>
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
-      <c r="Q15" s="41" t="s">
+      <c r="Q15" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42"/>
-      <c r="T15" s="43"/>
+      <c r="R15" s="44"/>
+      <c r="S15" s="44"/>
+      <c r="T15" s="39"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
     </row>
@@ -1485,7 +1521,7 @@
       <c r="V16" s="1"/>
     </row>
     <row r="17" spans="6:22" x14ac:dyDescent="0.2">
-      <c r="F17" s="34" t="s">
+      <c r="F17" s="45" t="s">
         <v>1</v>
       </c>
       <c r="G17" s="24">
@@ -1506,21 +1542,29 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="1"/>
-      <c r="O17" s="34" t="s">
+      <c r="O17" s="45" t="s">
         <v>1</v>
       </c>
       <c r="P17" s="24">
         <v>2</v>
       </c>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
+      <c r="Q17" s="9">
+        <v>14339</v>
+      </c>
+      <c r="R17" s="27">
+        <v>6503</v>
+      </c>
+      <c r="S17" s="9">
+        <v>4743</v>
+      </c>
+      <c r="T17" s="9">
+        <v>3433</v>
+      </c>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
     </row>
     <row r="18" spans="6:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F18" s="35"/>
+      <c r="F18" s="46"/>
       <c r="G18" s="7">
         <v>3</v>
       </c>
@@ -1539,19 +1583,27 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="1"/>
-      <c r="O18" s="35"/>
+      <c r="O18" s="46"/>
       <c r="P18" s="7">
         <v>3</v>
       </c>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="28"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
+      <c r="Q18" s="7">
+        <v>10307</v>
+      </c>
+      <c r="R18" s="28">
+        <v>5149</v>
+      </c>
+      <c r="S18" s="7">
+        <v>4061</v>
+      </c>
+      <c r="T18" s="7">
+        <v>2958</v>
+      </c>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
     </row>
     <row r="19" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F19" s="35"/>
+      <c r="F19" s="46"/>
       <c r="G19" s="23">
         <v>4</v>
       </c>
@@ -1570,19 +1622,27 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="1"/>
-      <c r="O19" s="35"/>
+      <c r="O19" s="46"/>
       <c r="P19" s="23">
         <v>4</v>
       </c>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="29"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="23"/>
+      <c r="Q19" s="23">
+        <v>10520</v>
+      </c>
+      <c r="R19" s="29">
+        <v>5240</v>
+      </c>
+      <c r="S19" s="23">
+        <v>4028</v>
+      </c>
+      <c r="T19" s="23">
+        <v>3006</v>
+      </c>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
     </row>
     <row r="20" spans="6:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="34" t="s">
+      <c r="F20" s="45" t="s">
         <v>5</v>
       </c>
       <c r="G20" s="10">
@@ -1603,21 +1663,29 @@
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="1"/>
-      <c r="O20" s="34" t="s">
+      <c r="O20" s="45" t="s">
         <v>5</v>
       </c>
       <c r="P20" s="10">
         <v>2</v>
       </c>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="30"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
+      <c r="Q20" s="10">
+        <v>14266</v>
+      </c>
+      <c r="R20" s="30">
+        <v>7101</v>
+      </c>
+      <c r="S20" s="10">
+        <v>4913</v>
+      </c>
+      <c r="T20" s="10">
+        <v>3578</v>
+      </c>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
     </row>
     <row r="21" spans="6:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="35"/>
+      <c r="F21" s="46"/>
       <c r="G21" s="7">
         <v>3</v>
       </c>
@@ -1636,19 +1704,27 @@
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="1"/>
-      <c r="O21" s="35"/>
+      <c r="O21" s="46"/>
       <c r="P21" s="7">
         <v>3</v>
       </c>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="28"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
+      <c r="Q21" s="7">
+        <v>12835</v>
+      </c>
+      <c r="R21" s="28">
+        <v>6174</v>
+      </c>
+      <c r="S21" s="7">
+        <v>4046</v>
+      </c>
+      <c r="T21" s="7">
+        <v>3331</v>
+      </c>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
     </row>
     <row r="22" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F22" s="36"/>
+      <c r="F22" s="47"/>
       <c r="G22" s="8">
         <v>4</v>
       </c>
@@ -1667,14 +1743,22 @@
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
       <c r="N22" s="1"/>
-      <c r="O22" s="36"/>
+      <c r="O22" s="47"/>
       <c r="P22" s="8">
         <v>4</v>
       </c>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="31"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="8"/>
+      <c r="Q22" s="8">
+        <v>13046</v>
+      </c>
+      <c r="R22" s="31">
+        <v>6267</v>
+      </c>
+      <c r="S22" s="8">
+        <v>4595</v>
+      </c>
+      <c r="T22" s="8">
+        <v>3374</v>
+      </c>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
     </row>
@@ -1776,48 +1860,48 @@
     <row r="28" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="37" t="s">
+      <c r="H28" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
-      <c r="M28" s="37"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="43"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
-      <c r="Q28" s="37" t="s">
+      <c r="Q28" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="R28" s="37"/>
-      <c r="S28" s="37"/>
-      <c r="T28" s="37"/>
-      <c r="U28" s="37"/>
-      <c r="V28" s="37"/>
+      <c r="R28" s="43"/>
+      <c r="S28" s="43"/>
+      <c r="T28" s="43"/>
+      <c r="U28" s="43"/>
+      <c r="V28" s="43"/>
     </row>
     <row r="29" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="38" t="s">
+      <c r="H29" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="40"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="41"/>
+      <c r="L29" s="41"/>
+      <c r="M29" s="42"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
-      <c r="Q29" s="38" t="s">
+      <c r="Q29" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="R29" s="39"/>
-      <c r="S29" s="39"/>
-      <c r="T29" s="39"/>
-      <c r="U29" s="39"/>
-      <c r="V29" s="40"/>
+      <c r="R29" s="41"/>
+      <c r="S29" s="41"/>
+      <c r="T29" s="41"/>
+      <c r="U29" s="41"/>
+      <c r="V29" s="42"/>
     </row>
     <row r="30" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F30" s="1"/>
@@ -1867,7 +1951,7 @@
       </c>
     </row>
     <row r="31" spans="6:22" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F31" s="34" t="s">
+      <c r="F31" s="45" t="s">
         <v>1</v>
       </c>
       <c r="G31" s="9">
@@ -1892,7 +1976,7 @@
         <v>29992</v>
       </c>
       <c r="N31" s="1"/>
-      <c r="O31" s="34" t="s">
+      <c r="O31" s="45" t="s">
         <v>1</v>
       </c>
       <c r="P31" s="9">
@@ -1918,7 +2002,7 @@
       </c>
     </row>
     <row r="32" spans="6:22" x14ac:dyDescent="0.2">
-      <c r="F32" s="35"/>
+      <c r="F32" s="46"/>
       <c r="G32" s="7">
         <v>3</v>
       </c>
@@ -1941,7 +2025,7 @@
         <v>22857</v>
       </c>
       <c r="N32" s="1"/>
-      <c r="O32" s="35"/>
+      <c r="O32" s="46"/>
       <c r="P32" s="7">
         <v>3</v>
       </c>
@@ -1965,7 +2049,7 @@
       </c>
     </row>
     <row r="33" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F33" s="35"/>
+      <c r="F33" s="46"/>
       <c r="G33" s="23">
         <v>4</v>
       </c>
@@ -1988,7 +2072,7 @@
         <v>29090</v>
       </c>
       <c r="N33" s="1"/>
-      <c r="O33" s="35"/>
+      <c r="O33" s="46"/>
       <c r="P33" s="23">
         <v>4</v>
       </c>
@@ -2012,7 +2096,7 @@
       </c>
     </row>
     <row r="34" spans="6:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F34" s="34" t="s">
+      <c r="F34" s="45" t="s">
         <v>5</v>
       </c>
       <c r="G34" s="10">
@@ -2037,7 +2121,7 @@
         <v>14893</v>
       </c>
       <c r="N34" s="1"/>
-      <c r="O34" s="34" t="s">
+      <c r="O34" s="45" t="s">
         <v>5</v>
       </c>
       <c r="P34" s="10">
@@ -2063,7 +2147,7 @@
       </c>
     </row>
     <row r="35" spans="6:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F35" s="35"/>
+      <c r="F35" s="46"/>
       <c r="G35" s="7">
         <v>3</v>
       </c>
@@ -2086,7 +2170,7 @@
         <v>11659</v>
       </c>
       <c r="N35" s="2"/>
-      <c r="O35" s="35"/>
+      <c r="O35" s="46"/>
       <c r="P35" s="7">
         <v>3</v>
       </c>
@@ -2110,7 +2194,7 @@
       </c>
     </row>
     <row r="36" spans="6:22" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F36" s="36"/>
+      <c r="F36" s="47"/>
       <c r="G36" s="8">
         <v>4</v>
       </c>
@@ -2133,7 +2217,7 @@
         <v>10564</v>
       </c>
       <c r="N36" s="2"/>
-      <c r="O36" s="36"/>
+      <c r="O36" s="47"/>
       <c r="P36" s="8">
         <v>4</v>
       </c>
@@ -2216,46 +2300,46 @@
     <row r="40" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="37" t="s">
+      <c r="H40" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="37"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43"/>
+      <c r="K40" s="43"/>
       <c r="L40" s="20"/>
       <c r="M40" s="20"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
-      <c r="Q40" s="37" t="s">
+      <c r="Q40" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="R40" s="37"/>
-      <c r="S40" s="37"/>
-      <c r="T40" s="37"/>
+      <c r="R40" s="43"/>
+      <c r="S40" s="43"/>
+      <c r="T40" s="43"/>
       <c r="U40" s="20"/>
       <c r="V40" s="20"/>
     </row>
     <row r="41" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="41" t="s">
+      <c r="H41" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="I41" s="42"/>
-      <c r="J41" s="42"/>
-      <c r="K41" s="43"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="44"/>
+      <c r="K41" s="39"/>
       <c r="L41" s="20"/>
       <c r="M41" s="20"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
-      <c r="Q41" s="41" t="s">
+      <c r="Q41" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="R41" s="42"/>
-      <c r="S41" s="42"/>
-      <c r="T41" s="43"/>
+      <c r="R41" s="44"/>
+      <c r="S41" s="44"/>
+      <c r="T41" s="39"/>
       <c r="U41" s="20"/>
       <c r="V41" s="20"/>
     </row>
@@ -2299,7 +2383,7 @@
       <c r="V42" s="4"/>
     </row>
     <row r="43" spans="6:22" x14ac:dyDescent="0.2">
-      <c r="F43" s="34" t="s">
+      <c r="F43" s="45" t="s">
         <v>1</v>
       </c>
       <c r="G43" s="22">
@@ -2320,7 +2404,7 @@
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
       <c r="N43" s="1"/>
-      <c r="O43" s="34" t="s">
+      <c r="O43" s="45" t="s">
         <v>1</v>
       </c>
       <c r="P43" s="24">
@@ -2342,7 +2426,7 @@
       <c r="V43" s="4"/>
     </row>
     <row r="44" spans="6:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F44" s="35"/>
+      <c r="F44" s="46"/>
       <c r="G44" s="7">
         <v>3</v>
       </c>
@@ -2361,7 +2445,7 @@
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
       <c r="N44" s="1"/>
-      <c r="O44" s="35"/>
+      <c r="O44" s="46"/>
       <c r="P44" s="7">
         <v>3</v>
       </c>
@@ -2381,7 +2465,7 @@
       <c r="V44" s="4"/>
     </row>
     <row r="45" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F45" s="35"/>
+      <c r="F45" s="46"/>
       <c r="G45" s="23">
         <v>4</v>
       </c>
@@ -2400,7 +2484,7 @@
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
       <c r="N45" s="1"/>
-      <c r="O45" s="35"/>
+      <c r="O45" s="46"/>
       <c r="P45" s="23">
         <v>4</v>
       </c>
@@ -2420,7 +2504,7 @@
       <c r="V45" s="4"/>
     </row>
     <row r="46" spans="6:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F46" s="34" t="s">
+      <c r="F46" s="45" t="s">
         <v>5</v>
       </c>
       <c r="G46" s="10">
@@ -2441,7 +2525,7 @@
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
       <c r="N46" s="1"/>
-      <c r="O46" s="34" t="s">
+      <c r="O46" s="45" t="s">
         <v>5</v>
       </c>
       <c r="P46" s="10">
@@ -2463,7 +2547,7 @@
       <c r="V46" s="4"/>
     </row>
     <row r="47" spans="6:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F47" s="35"/>
+      <c r="F47" s="46"/>
       <c r="G47" s="7">
         <v>3</v>
       </c>
@@ -2482,7 +2566,7 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
       <c r="N47" s="1"/>
-      <c r="O47" s="35"/>
+      <c r="O47" s="46"/>
       <c r="P47" s="7">
         <v>3</v>
       </c>
@@ -2502,7 +2586,7 @@
       <c r="V47" s="4"/>
     </row>
     <row r="48" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F48" s="36"/>
+      <c r="F48" s="47"/>
       <c r="G48" s="8">
         <v>4</v>
       </c>
@@ -2521,7 +2605,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="1"/>
-      <c r="O48" s="36"/>
+      <c r="O48" s="47"/>
       <c r="P48" s="8">
         <v>4</v>
       </c>
@@ -2599,16 +2683,12 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="H3:M3"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="Q2:V2"/>
-    <mergeCell ref="Q3:V3"/>
-    <mergeCell ref="Q14:T14"/>
-    <mergeCell ref="Q15:T15"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="O43:O45"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="O8:O10"/>
+    <mergeCell ref="F17:F19"/>
     <mergeCell ref="O46:O48"/>
     <mergeCell ref="F43:F45"/>
     <mergeCell ref="F46:F48"/>
@@ -2624,14 +2704,18 @@
     <mergeCell ref="H29:M29"/>
     <mergeCell ref="F34:F36"/>
     <mergeCell ref="F31:F33"/>
+    <mergeCell ref="Q14:T14"/>
+    <mergeCell ref="Q15:T15"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="O43:O45"/>
     <mergeCell ref="O17:O19"/>
     <mergeCell ref="O20:O22"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="O8:O10"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="Q2:V2"/>
+    <mergeCell ref="Q3:V3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added report and submission zip file
</commit_message>
<xml_diff>
--- a/HMMs analysis.xlsx
+++ b/HMMs analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="33520" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -106,6 +106,12 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -926,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2717,6 +2723,12 @@
     <mergeCell ref="Q2:V2"/>
     <mergeCell ref="Q3:V3"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="98" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <colBreaks count="2" manualBreakCount="2">
+    <brk id="6" max="1048575" man="1"/>
+    <brk id="14" max="1048575" man="1"/>
+  </colBreaks>
 </worksheet>
 </file>
</xml_diff>